<commit_message>
kosten en baten / logboek
begin gemaakt aan kosten en baten en mn logboek bijgewerkt
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek Kevin Nunes da Silva.xlsx
+++ b/Documents/Logboeken/Logboek Kevin Nunes da Silva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Worst Hooker\Documents\GitHub\project_fifa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\GitHub\project_fifa\Documents\Logboeken\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -95,6 +95,27 @@
   </si>
   <si>
     <t>14:15/15:30</t>
+  </si>
+  <si>
+    <t>week 1</t>
+  </si>
+  <si>
+    <t>14:20/15:00</t>
+  </si>
+  <si>
+    <t>kosten en baten begin gemaakt</t>
+  </si>
+  <si>
+    <t>dinsdag</t>
+  </si>
+  <si>
+    <t>woensdag</t>
+  </si>
+  <si>
+    <t>13:00/13:50</t>
+  </si>
+  <si>
+    <t>begonnen met de groep aan het plan van aanpak</t>
   </si>
 </sst>
 </file>
@@ -467,14 +488,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,6 +539,9 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
@@ -531,6 +556,9 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
@@ -545,6 +573,9 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -559,6 +590,9 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -567,6 +601,40 @@
       </c>
       <c r="G10" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>